<commit_message>
Cambio limpieza de formato
</commit_message>
<xml_diff>
--- a/Sistemas/CCFN-D008-A13-R00 FORMATO COMPARATIVO DE COTIZACIONES.xlsx
+++ b/Sistemas/CCFN-D008-A13-R00 FORMATO COMPARATIVO DE COTIZACIONES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\OneDrive\CCFN\Documentacion\Formatos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IT\Documents\GitHub\Formatos\Sistemas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Empresa</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Bicom</t>
   </si>
   <si>
-    <t>CL-5500</t>
-  </si>
-  <si>
-    <t>Tarjeta Madre Principal CL-5500</t>
-  </si>
-  <si>
     <t>iva M.N.</t>
   </si>
   <si>
@@ -81,25 +75,7 @@
     <t>Comparativo de Cotizaciones CCFN</t>
   </si>
   <si>
-    <t>CAS</t>
-  </si>
-  <si>
-    <t>Tarjeta Principal de Bascula</t>
-  </si>
-  <si>
-    <t>Tarjeta Principal, Procesador</t>
-  </si>
-  <si>
     <t>Entrega</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>5 Dias</t>
-  </si>
-  <si>
-    <t>3 Dias</t>
   </si>
   <si>
     <t>Nombre y Firma</t>
@@ -1127,7 +1103,7 @@
   <dimension ref="C3:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,11 +1125,11 @@
       <c r="C3" s="43"/>
       <c r="D3" s="44"/>
       <c r="E3" s="38" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F3" s="38"/>
       <c r="G3" s="39" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H3" s="40"/>
       <c r="I3" s="43"/>
@@ -1169,7 +1145,7 @@
       <c r="E4" s="38"/>
       <c r="F4" s="38"/>
       <c r="G4" s="41" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H4" s="42"/>
       <c r="I4" s="45"/>
@@ -1185,7 +1161,7 @@
       <c r="E5" s="38"/>
       <c r="F5" s="38"/>
       <c r="G5" s="41" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H5" s="42"/>
       <c r="I5" s="47"/>
@@ -1225,7 +1201,7 @@
     </row>
     <row r="8" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -1270,53 +1246,45 @@
         <v>5</v>
       </c>
       <c r="H10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="N10" s="21" t="s">
         <v>15</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="N10" s="21" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="3:14" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
       <c r="H11" s="10">
-        <v>5360</v>
+        <v>0</v>
       </c>
       <c r="I11" s="10">
         <f>H11*0.16</f>
-        <v>857.6</v>
+        <v>0</v>
       </c>
       <c r="J11" s="10">
         <f>H11+I11</f>
-        <v>6217.6</v>
+        <v>0</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="3">
@@ -1325,28 +1293,18 @@
       </c>
       <c r="M11" s="16">
         <f>J11+L11</f>
-        <v>6217.6</v>
-      </c>
-      <c r="N11" s="20" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="11">
         <v>0</v>
       </c>
@@ -1359,36 +1317,26 @@
         <v>0</v>
       </c>
       <c r="K12" s="11">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="L12" s="11">
         <f>K12*1.16</f>
-        <v>290</v>
+        <v>0</v>
       </c>
       <c r="M12" s="17">
         <f>J12+L12</f>
-        <v>290</v>
-      </c>
-      <c r="N12" s="18" t="s">
-        <v>23</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="3">
         <v>0</v>
       </c>
@@ -1401,19 +1349,17 @@
         <v>0</v>
       </c>
       <c r="K13" s="3">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="L13" s="3">
         <f>K13*1.16</f>
-        <v>290</v>
+        <v>0</v>
       </c>
       <c r="M13" s="16">
         <f>K13+L13</f>
-        <v>540</v>
-      </c>
-      <c r="N13" s="19" t="s">
-        <v>22</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="N13" s="19"/>
     </row>
     <row r="14" spans="3:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
@@ -1469,47 +1415,47 @@
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D22" s="22" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="G22" s="22" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D23" s="24" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G23" s="24" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D24" s="24" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" s="26" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D26" s="25"/>
       <c r="G26" s="26" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="J26" s="26" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="K26" s="26"/>
     </row>
@@ -1541,67 +1487,67 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>